<commit_message>
add new test patients
</commit_message>
<xml_diff>
--- a/extras/TestData_P4_C5_002.1.xlsx
+++ b/extras/TestData_P4_C5_002.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ablack/darwin/PregnancyIdentifier/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A24F171-A19F-FE44-B9B9-FA7F10A050A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CA57B7-B6BC-F742-8B9D-D49531BC5671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4220" windowWidth="34200" windowHeight="12660" activeTab="2" xr2:uid="{2624F3FA-1896-E346-B17D-1AF481078F66}"/>
+    <workbookView xWindow="300" yWindow="660" windowWidth="34200" windowHeight="12660" activeTab="5" xr2:uid="{2624F3FA-1896-E346-B17D-1AF481078F66}"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="132">
   <si>
     <t>person_id</t>
   </si>
@@ -475,6 +475,12 @@
   </si>
   <si>
     <t>condition_source_value</t>
+  </si>
+  <si>
+    <t>Gestation period, 39 weeks</t>
+  </si>
+  <si>
+    <t>Maternal postnatal 6 week examination</t>
   </si>
 </sst>
 </file>
@@ -612,7 +618,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -693,6 +699,12 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1029,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A1C072-644C-1A47-9B0F-C596ED60D337}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1661,6 +1673,86 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>8532</v>
+      </c>
+      <c r="C32">
+        <v>1990</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>8532</v>
+      </c>
+      <c r="C33">
+        <v>1990</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>8532</v>
+      </c>
+      <c r="C34">
+        <v>1990</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>8532</v>
+      </c>
+      <c r="C35">
+        <v>1990</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2242,10 +2334,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00E21BF-3345-8E43-B920-A246747D8F60}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="158" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A26" zoomScale="158" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2783,6 +2875,74 @@
         <v>12</v>
       </c>
     </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>35</v>
+      </c>
+      <c r="C32" s="11">
+        <v>40909</v>
+      </c>
+      <c r="D32" s="11">
+        <v>45657</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>36</v>
+      </c>
+      <c r="C33" s="11">
+        <v>40909</v>
+      </c>
+      <c r="D33" s="11">
+        <v>45657</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>37</v>
+      </c>
+      <c r="C34" s="11">
+        <v>40909</v>
+      </c>
+      <c r="D34" s="11">
+        <v>45657</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>38</v>
+      </c>
+      <c r="C35" s="11">
+        <v>40909</v>
+      </c>
+      <c r="D35" s="11">
+        <v>45657</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E17" xr:uid="{F00E21BF-3345-8E43-B920-A246747D8F60}"/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2794,10 +2954,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556FAEDB-4FE7-8849-9EBA-5154A838789B}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:U59"/>
+  <dimension ref="A1:U66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4399,6 +4559,188 @@
       </c>
       <c r="H59" s="27" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="17">
+      <c r="A60" s="19">
+        <v>66</v>
+      </c>
+      <c r="B60" s="19">
+        <v>35</v>
+      </c>
+      <c r="C60" s="33">
+        <v>444098</v>
+      </c>
+      <c r="D60" s="34">
+        <v>45280</v>
+      </c>
+      <c r="E60" s="19">
+        <v>32817</v>
+      </c>
+      <c r="F60" s="19">
+        <v>0</v>
+      </c>
+      <c r="G60" s="19">
+        <v>0</v>
+      </c>
+      <c r="H60" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="17">
+      <c r="A61" s="19">
+        <v>67</v>
+      </c>
+      <c r="B61" s="19">
+        <v>36</v>
+      </c>
+      <c r="C61" s="27">
+        <v>4014295</v>
+      </c>
+      <c r="D61" s="28">
+        <v>45280</v>
+      </c>
+      <c r="E61" s="19">
+        <v>32817</v>
+      </c>
+      <c r="F61" s="19">
+        <v>0</v>
+      </c>
+      <c r="G61" s="19">
+        <v>0</v>
+      </c>
+      <c r="H61" s="27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="17">
+      <c r="A62" s="3">
+        <v>68</v>
+      </c>
+      <c r="B62" s="3">
+        <v>36</v>
+      </c>
+      <c r="C62" s="27">
+        <v>444098</v>
+      </c>
+      <c r="D62" s="28">
+        <v>45280</v>
+      </c>
+      <c r="E62" s="3">
+        <v>32817</v>
+      </c>
+      <c r="F62" s="3">
+        <v>0</v>
+      </c>
+      <c r="G62" s="3">
+        <v>0</v>
+      </c>
+      <c r="H62" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="17">
+      <c r="A63" s="19">
+        <v>69</v>
+      </c>
+      <c r="B63" s="19">
+        <v>37</v>
+      </c>
+      <c r="C63" s="27">
+        <v>4014295</v>
+      </c>
+      <c r="D63" s="28">
+        <v>45280</v>
+      </c>
+      <c r="E63" s="19">
+        <v>32817</v>
+      </c>
+      <c r="F63" s="19">
+        <v>0</v>
+      </c>
+      <c r="G63" s="19">
+        <v>0</v>
+      </c>
+      <c r="H63" s="27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="17">
+      <c r="A64" s="19">
+        <v>70</v>
+      </c>
+      <c r="B64" s="19">
+        <v>37</v>
+      </c>
+      <c r="C64" s="13">
+        <v>435655</v>
+      </c>
+      <c r="D64" s="28">
+        <v>45273</v>
+      </c>
+      <c r="E64" s="19">
+        <v>32817</v>
+      </c>
+      <c r="F64" s="19">
+        <v>0</v>
+      </c>
+      <c r="G64" s="19">
+        <v>0</v>
+      </c>
+      <c r="H64" s="27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="17">
+      <c r="A65" s="3">
+        <v>71</v>
+      </c>
+      <c r="B65" s="3">
+        <v>38</v>
+      </c>
+      <c r="C65" s="27">
+        <v>444098</v>
+      </c>
+      <c r="D65" s="28">
+        <v>45280</v>
+      </c>
+      <c r="E65" s="3">
+        <v>32817</v>
+      </c>
+      <c r="F65" s="3">
+        <v>0</v>
+      </c>
+      <c r="G65" s="3">
+        <v>0</v>
+      </c>
+      <c r="H65" s="27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="17">
+      <c r="A66" s="19">
+        <v>72</v>
+      </c>
+      <c r="B66" s="19">
+        <v>38</v>
+      </c>
+      <c r="C66" s="27">
+        <v>4014295</v>
+      </c>
+      <c r="D66" s="28">
+        <v>45266</v>
+      </c>
+      <c r="E66" s="19">
+        <v>32817</v>
+      </c>
+      <c r="F66" s="19">
+        <v>0</v>
+      </c>
+      <c r="G66" s="19">
+        <v>0</v>
+      </c>
+      <c r="H66" s="27" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -4487,9 +4829,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85A45E38-DECC-8A44-B5EF-C13538335272}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -4618,10 +4962,31 @@
         <v>125</v>
       </c>
     </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>35</v>
+      </c>
+      <c r="C7" s="13">
+        <v>4297233</v>
+      </c>
+      <c r="D7" s="28">
+        <v>45328</v>
+      </c>
+      <c r="E7" s="3">
+        <v>32817</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>131</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" location="/concept/2211747" display="https://atlas.darwin-eu.org/ - /concept/2211747" xr:uid="{89C52AD5-15F6-6C4D-97F8-9BCE6319924F}"/>
     <hyperlink ref="F2" r:id="rId2" location="/concept/2211751" display="https://atlas.darwin-eu.org/ - /concept/2211751" xr:uid="{DBFBC6DA-9ECD-A143-B1B4-5FD1CAACC124}"/>
+    <hyperlink ref="F7" r:id="rId3" location="/concept/4297233" display="https://atlas.darwin-eu.org/ - /concept/4297233" xr:uid="{1F0988C5-C285-9D46-8CA0-FC2BDA22CA43}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4631,8 +4996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C4A2F6-3FDC-164F-B9B8-140301E5C5A8}">
   <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -5258,10 +5623,10 @@
       <c r="B11">
         <v>21</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="36">
         <v>3036000</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="25">
         <v>45179</v>
       </c>
       <c r="G11">
@@ -5272,16 +5637,16 @@
       </c>
     </row>
     <row r="12" spans="1:20" s="5" customFormat="1">
-      <c r="A12" s="3">
+      <c r="A12" s="35">
         <v>62</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="35">
         <v>34</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="36">
         <v>3036000</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="25">
         <v>45260</v>
       </c>
       <c r="E12" s="3"/>
@@ -6398,9 +6763,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6542,26 +6910,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B74C39-E305-437B-89E5-691639CCCAB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1BB2D99-B90A-4F2C-B88E-D2F6417F47F2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2f696df8-7461-455e-9bf1-ef56149775f2"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6585,9 +6942,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1BB2D99-B90A-4F2C-B88E-D2F6417F47F2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01B74C39-E305-437B-89E5-691639CCCAB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2f696df8-7461-455e-9bf1-ef56149775f2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add attrition, logging, tests
</commit_message>
<xml_diff>
--- a/extras/TestData_P4_C5_002.1.xlsx
+++ b/extras/TestData_P4_C5_002.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ablack/darwin/PregnancyIdentifier/extras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CA57B7-B6BC-F742-8B9D-D49531BC5671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A235FF58-43C5-1448-9140-9BB346C29934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="660" windowWidth="34200" windowHeight="12660" activeTab="5" xr2:uid="{2624F3FA-1896-E346-B17D-1AF481078F66}"/>
+    <workbookView xWindow="780" yWindow="6000" windowWidth="34200" windowHeight="12660" activeTab="5" xr2:uid="{2624F3FA-1896-E346-B17D-1AF481078F66}"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="134">
   <si>
     <t>person_id</t>
   </si>
@@ -481,6 +481,12 @@
   </si>
   <si>
     <t>Maternal postnatal 6 week examination</t>
+  </si>
+  <si>
+    <t>Pregnancy</t>
+  </si>
+  <si>
+    <t>Complication occurring during labor and delivery</t>
   </si>
 </sst>
 </file>
@@ -577,7 +583,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -613,12 +619,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD9D9D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -705,6 +722,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1041,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A1C072-644C-1A47-9B0F-C596ED60D337}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:F35"/>
+      <selection activeCell="A36" sqref="A1:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1753,6 +1773,46 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>8532</v>
+      </c>
+      <c r="C36">
+        <v>1990</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>8532</v>
+      </c>
+      <c r="C37">
+        <v>1990</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2334,10 +2394,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00E21BF-3345-8E43-B920-A246747D8F60}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView topLeftCell="A26" zoomScale="158" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:E35"/>
+      <selection activeCell="A36" sqref="A36:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2943,6 +3003,40 @@
         <v>12</v>
       </c>
     </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>39</v>
+      </c>
+      <c r="C36" s="11">
+        <v>40909</v>
+      </c>
+      <c r="D36" s="11">
+        <v>45657</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>40</v>
+      </c>
+      <c r="C37" s="11">
+        <v>40909</v>
+      </c>
+      <c r="D37" s="11">
+        <v>45657</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E17" xr:uid="{F00E21BF-3345-8E43-B920-A246747D8F60}"/>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2954,10 +3048,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{556FAEDB-4FE7-8849-9EBA-5154A838789B}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:U66"/>
+  <dimension ref="A1:U68"/>
   <sheetViews>
     <sheetView topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:H66"/>
+      <selection activeCell="A67" sqref="A67:H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4741,6 +4835,58 @@
       </c>
       <c r="H66" s="27" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="17">
+      <c r="A67" s="3">
+        <v>73</v>
+      </c>
+      <c r="B67" s="3">
+        <v>39</v>
+      </c>
+      <c r="C67" s="3">
+        <v>4299535</v>
+      </c>
+      <c r="D67" s="10">
+        <v>43879</v>
+      </c>
+      <c r="E67" s="3">
+        <v>32817</v>
+      </c>
+      <c r="F67" s="3">
+        <v>0</v>
+      </c>
+      <c r="G67" s="3">
+        <v>0</v>
+      </c>
+      <c r="H67" s="37" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="17">
+      <c r="A68" s="3">
+        <v>74</v>
+      </c>
+      <c r="B68" s="3">
+        <v>40</v>
+      </c>
+      <c r="C68" s="3">
+        <v>440795</v>
+      </c>
+      <c r="D68" s="28">
+        <v>43857</v>
+      </c>
+      <c r="E68" s="3">
+        <v>32817</v>
+      </c>
+      <c r="F68" s="3">
+        <v>0</v>
+      </c>
+      <c r="G68" s="3">
+        <v>0</v>
+      </c>
+      <c r="H68" s="37" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -4994,10 +5140,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C4A2F6-3FDC-164F-B9B8-140301E5C5A8}">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -5653,6 +5799,237 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="27"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>39</v>
+      </c>
+      <c r="C13" s="12">
+        <v>3012266</v>
+      </c>
+      <c r="D13" s="25">
+        <v>43879</v>
+      </c>
+      <c r="E13" s="26">
+        <v>43879.833333333336</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13">
+        <v>32585</v>
+      </c>
+      <c r="H13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>8511</v>
+      </c>
+      <c r="N13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>39</v>
+      </c>
+      <c r="C14" s="12">
+        <v>3012266</v>
+      </c>
+      <c r="D14" s="25">
+        <v>44116</v>
+      </c>
+      <c r="E14" s="26">
+        <v>44116.833333333336</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14">
+        <v>32585</v>
+      </c>
+      <c r="H14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14">
+        <v>42</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>8511</v>
+      </c>
+      <c r="N14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15" s="12">
+        <v>3012266</v>
+      </c>
+      <c r="D15" s="25">
+        <v>43681</v>
+      </c>
+      <c r="E15" s="26">
+        <v>43681.833333333336</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15">
+        <v>32585</v>
+      </c>
+      <c r="H15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15">
+        <v>17</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>8511</v>
+      </c>
+      <c r="N15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>40</v>
+      </c>
+      <c r="C16" s="12">
+        <v>3012266</v>
+      </c>
+      <c r="D16" s="25">
+        <v>43797</v>
+      </c>
+      <c r="E16" s="26">
+        <v>43797.833333333336</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16">
+        <v>32585</v>
+      </c>
+      <c r="H16" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16">
+        <v>35</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>8511</v>
+      </c>
+      <c r="N16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17" s="12">
+        <v>4091201</v>
+      </c>
+      <c r="D17" s="25">
+        <v>43867</v>
+      </c>
+      <c r="E17" s="26">
+        <v>43867.833333333336</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17">
+        <v>32585</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>7</v>
+      </c>
+      <c r="M17">
+        <v>10</v>
+      </c>
+      <c r="N17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>40</v>
+      </c>
+      <c r="C18" s="12">
+        <v>3012266</v>
+      </c>
+      <c r="D18" s="25">
+        <v>43882</v>
+      </c>
+      <c r="E18" s="26">
+        <v>43882.833333333336</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18">
+        <v>32585</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18">
+        <v>42</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>8511</v>
+      </c>
+      <c r="N18" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>